<commit_message>
add script to plot distribution of turn features
</commit_message>
<xml_diff>
--- a/datalists/npr1_40_list.xlsx
+++ b/datalists/npr1_40_list.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>/data2/shared/data/Results/recording28.6g100-500/recording28.6g_X1_skeletons.hdf5</t>
   </si>
@@ -23,6 +23,9 @@
   </si>
   <si>
     <t>/data2/shared/data/Results/recording31.2g100-500/recording31.2g_X1_skeletons.hdf5</t>
+  </si>
+  <si>
+    <t>/data2/shared/data/Results/recording32.6g100-200/recording32.6g_X1_skeletons.hdf5</t>
   </si>
   <si>
     <t>/data2/shared/data/Results/recording33.6g100-200/recording33.6g_X1_skeletons.hdf5</t>
@@ -143,7 +146,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>9000.0</v>
+        <v>3100.0</v>
       </c>
     </row>
     <row r="6">
@@ -151,7 +154,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>6000.0</v>
+        <v>9000.0</v>
       </c>
     </row>
     <row r="7">
@@ -159,7 +162,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>3000.0</v>
+        <v>6000.0</v>
       </c>
     </row>
     <row r="8">
@@ -167,7 +170,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>14000.0</v>
+        <v>3000.0</v>
       </c>
     </row>
     <row r="9">
@@ -175,7 +178,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>7500.0</v>
+        <v>14000.0</v>
       </c>
     </row>
     <row r="10">
@@ -183,7 +186,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>13500.0</v>
+        <v>7500.0</v>
       </c>
     </row>
     <row r="11">
@@ -191,6 +194,14 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
+        <v>13500.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
         <v>7700.0</v>
       </c>
     </row>

</xml_diff>